<commit_message>
changes matrix. added new chapter for testing.
</commit_message>
<xml_diff>
--- a/Matrix _NEU.xlsx
+++ b/Matrix _NEU.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Kosten</t>
   </si>
@@ -68,12 +68,39 @@
     <t>klare Sprache</t>
   </si>
   <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>keine</t>
+  </si>
+  <si>
+    <t>gering</t>
+  </si>
+  <si>
     <t>keine Einschränkung</t>
   </si>
   <si>
+    <t>teils</t>
+  </si>
+  <si>
     <t>nein</t>
   </si>
   <si>
+    <t>mittel</t>
+  </si>
+  <si>
+    <t>beschränkt</t>
+  </si>
+  <si>
+    <t>hoch</t>
+  </si>
+  <si>
+    <t>sehr hoch</t>
+  </si>
+  <si>
+    <t>messbare Gehirnsignale über 3.5 Hz</t>
+  </si>
+  <si>
     <t>keine Produkte am Markt</t>
   </si>
   <si>
@@ -86,9 +113,15 @@
     <t>Kontrolle über Muskelan- und entspannungen</t>
   </si>
   <si>
+    <t>laut und deutlich sprechen, normale Sprechgeschwindigkeit, keine zu Große Distanz zum Mikrophon</t>
+  </si>
+  <si>
     <t>Laborsetting</t>
   </si>
   <si>
+    <t>gering (Gewicht des Joysticks)</t>
+  </si>
+  <si>
     <t>sehr gering (Gewicht der Elektroden)</t>
   </si>
   <si>
@@ -149,9 +182,6 @@
     <t>312g bis 3.8kg</t>
   </si>
   <si>
-    <t>gerin (Gewicht des Joysticks)</t>
-  </si>
-  <si>
     <t>Wartung, wenn sich die Stimme verändert</t>
   </si>
   <si>
@@ -159,6 +189,21 @@
   </si>
   <si>
     <t>Selbssttändige Aktivierung der Gehirnsignale</t>
+  </si>
+  <si>
+    <t>intuitiv</t>
+  </si>
+  <si>
+    <t>gewöhungsbedürftig</t>
+  </si>
+  <si>
+    <t>Brille, unterschiedliche Profile</t>
+  </si>
+  <si>
+    <t>Genaue Anpassung bei ruckartigen Bewegungen</t>
+  </si>
+  <si>
+    <t>Genaue Positionierung der Elektroden</t>
   </si>
 </sst>
 </file>
@@ -218,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -255,6 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,25 +617,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -604,10 +650,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -615,21 +661,21 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -638,22 +684,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -661,22 +707,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -687,49 +733,49 @@
         <v>250</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>1</v>
@@ -747,32 +793,122 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed test chapter. finalized matrix. added content to comparrison.
</commit_message>
<xml_diff>
--- a/Matrix _NEU.xlsx
+++ b/Matrix _NEU.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>Kosten</t>
   </si>
@@ -74,9 +74,6 @@
     <t>keine</t>
   </si>
   <si>
-    <t>gering</t>
-  </si>
-  <si>
     <t>keine Einschränkung</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>nein</t>
   </si>
   <si>
-    <t>mittel</t>
-  </si>
-  <si>
     <t>beschränkt</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>messbare Gehirnsignale über 3.5 Hz</t>
   </si>
   <si>
-    <t>keine Produkte am Markt</t>
-  </si>
-  <si>
     <t>kontrollierte Augenbewegungen</t>
   </si>
   <si>
@@ -204,6 +195,9 @@
   </si>
   <si>
     <t>Genaue Positionierung der Elektroden</t>
+  </si>
+  <si>
+    <t>niedrig</t>
   </si>
 </sst>
 </file>
@@ -237,18 +231,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -295,9 +283,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -650,10 +635,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -661,19 +646,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>13</v>
@@ -683,23 +668,23 @@
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>42</v>
+      <c r="B3" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -707,22 +692,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -733,49 +718,49 @@
         <v>250</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="7">
+        <v>720</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="E6" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>1</v>
@@ -793,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -801,22 +786,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="13" t="s">
         <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -824,22 +809,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -847,22 +832,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -870,45 +855,45 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="14" t="s">
-        <v>24</v>
+      <c r="G14" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rewrote a bunch of stuff.
</commit_message>
<xml_diff>
--- a/Matrix _NEU.xlsx
+++ b/Matrix _NEU.xlsx
@@ -107,15 +107,9 @@
     <t>laut und deutlich sprechen, normale Sprechgeschwindigkeit, keine zu Große Distanz zum Mikrophon</t>
   </si>
   <si>
-    <t>Laborsetting</t>
-  </si>
-  <si>
     <t>gering (Gewicht des Joysticks)</t>
   </si>
   <si>
-    <t>sehr gering (Gewicht der Elektroden)</t>
-  </si>
-  <si>
     <t>Myo-Armband: 11,9 x 7,4 x 10,4 cm</t>
   </si>
   <si>
@@ -152,27 +146,18 @@
     <t>drinnen</t>
   </si>
   <si>
-    <t>Laborsetting, Myo-Armband keine Einschränkung</t>
-  </si>
-  <si>
     <t>richtet sich nach Mikrophon und Interaktionsgerät</t>
   </si>
   <si>
     <t>richtet sich nach Interaktionsgerät</t>
   </si>
   <si>
-    <t>sehr klein (Größe der Elektroden)</t>
-  </si>
-  <si>
     <t>Fausgroß und größer</t>
   </si>
   <si>
     <t>kein zusätzliches Gewicht</t>
   </si>
   <si>
-    <t>312g bis 3.8kg</t>
-  </si>
-  <si>
     <t>Wartung, wenn sich die Stimme verändert</t>
   </si>
   <si>
@@ -198,6 +183,21 @@
   </si>
   <si>
     <t>niedrig</t>
+  </si>
+  <si>
+    <t>EPOC+: 540g</t>
+  </si>
+  <si>
+    <t>EPOC+ keine Einschränkung</t>
+  </si>
+  <si>
+    <t>Myo-Armband keine Einschränkung</t>
+  </si>
+  <si>
+    <t>EPOC+: 23 x 38 x 38 cm</t>
+  </si>
+  <si>
+    <t>312g bis 8.9kg</t>
   </si>
 </sst>
 </file>
@@ -251,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -286,6 +286,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +606,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -635,10 +638,10 @@
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -646,19 +649,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>13</v>
@@ -669,16 +672,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" s="7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>18</v>
@@ -692,25 +695,25 @@
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -718,13 +721,13 @@
         <v>250</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
@@ -733,34 +736,34 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="7">
+        <v>32</v>
+      </c>
+      <c r="B6" s="14">
         <v>720</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>1</v>
@@ -778,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -789,13 +792,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>17</v>
@@ -812,19 +815,19 @@
         <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -835,19 +838,19 @@
         <v>16</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -864,18 +867,18 @@
         <v>21</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
@@ -884,10 +887,10 @@
         <v>20</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>14</v>

</xml_diff>